<commit_message>
a pure Go VRF library is used in distributed experiment, here we have a fixed set of 4 IPs (VMs): starting from 192.168.3.220 to 192.168.3.223
from https://github.com/tmc/go-algorand/tree/purego-vrf
it is not merged into the master branch but still! it is one of the branches in Algorand.
</commit_message>
<xml_diff>
--- a/simulation/manage/simulation/mainchainbc.xlsx
+++ b/simulation/manage/simulation/mainchainbc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Server's Info</t>
   </si>
@@ -52,39 +52,6 @@
     <t>108</t>
   </si>
   <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
     <t>ServAgrDuration</t>
   </si>
   <si>
@@ -115,69 +82,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>StartedMCRoundNumber</t>
   </si>
   <si>
@@ -235,126 +139,6 @@
     <t>8987300396532588544</t>
   </si>
   <si>
-    <t>8980596437439105024</t>
-  </si>
-  <si>
-    <t>9006348376912575488</t>
-  </si>
-  <si>
-    <t>8988108343805682688</t>
-  </si>
-  <si>
-    <t>9019366186754210816</t>
-  </si>
-  <si>
-    <t>9006399876409530368</t>
-  </si>
-  <si>
-    <t>8993527267649944576</t>
-  </si>
-  <si>
-    <t>9005071899709859840</t>
-  </si>
-  <si>
-    <t>8982281333360569344</t>
-  </si>
-  <si>
-    <t>8989397569801741312</t>
-  </si>
-  <si>
-    <t>8999863785305648128</t>
-  </si>
-  <si>
-    <t>8994508046559886336</t>
-  </si>
-  <si>
-    <t>9015274292697842688</t>
-  </si>
-  <si>
-    <t>8989218251278460928</t>
-  </si>
-  <si>
-    <t>8991375068639620096</t>
-  </si>
-  <si>
-    <t>8994858503169117184</t>
-  </si>
-  <si>
-    <t>9002029969178644480</t>
-  </si>
-  <si>
-    <t>8995888749969917952</t>
-  </si>
-  <si>
-    <t>9008017166844525568</t>
-  </si>
-  <si>
-    <t>8997764116485407744</t>
-  </si>
-  <si>
-    <t>8993153707115029504</t>
-  </si>
-  <si>
-    <t>9002392585653391360</t>
-  </si>
-  <si>
-    <t>8995366556940910592</t>
-  </si>
-  <si>
-    <t>8997645790738826240</t>
-  </si>
-  <si>
-    <t>8998002122504554496</t>
-  </si>
-  <si>
-    <t>9003022074279255040</t>
-  </si>
-  <si>
-    <t>8998322046631143424</t>
-  </si>
-  <si>
-    <t>9001319025218248704</t>
-  </si>
-  <si>
-    <t>9002810339327276032</t>
-  </si>
-  <si>
-    <t>8998768633299628032</t>
-  </si>
-  <si>
-    <t>9011509607471220736</t>
-  </si>
-  <si>
-    <t>8993254617337384960</t>
-  </si>
-  <si>
-    <t>9000642050566681600</t>
-  </si>
-  <si>
-    <t>9006986069140862976</t>
-  </si>
-  <si>
-    <t>9006297465221599232</t>
-  </si>
-  <si>
-    <t>9002826980737875968</t>
-  </si>
-  <si>
-    <t>8995599128832134144</t>
-  </si>
-  <si>
-    <t>8991506204024881152</t>
-  </si>
-  <si>
-    <t>8993944641725438976</t>
-  </si>
-  <si>
-    <t>9004230546483422208</t>
-  </si>
-  <si>
-    <t>8996655111059198976</t>
-  </si>
-  <si>
     <t>Round#</t>
   </si>
   <si>
@@ -403,7 +187,7 @@
     <t>BlockSpaceFull</t>
   </si>
   <si>
-    <t>4e07408562bedb8b60ce05c1decfe3ad16b72230967de01f640b7e4729b49fce</t>
+    <t>4b227777d4dd1fc61c6f884f48641d02b4d121d3fd328cb08b5531fcacdabf8a</t>
   </si>
   <si>
     <t>Overall#RegPay-TX</t>
@@ -770,14 +554,14 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1482,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1496,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1510,7 +1294,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1524,7 +1308,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1538,7 +1322,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1552,7 +1336,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1566,7 +1350,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1580,7 +1364,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1594,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1608,572 +1392,12 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="F51">
         <v>0</v>
       </c>
     </row>
@@ -2201,19 +1425,19 @@
   <sheetData>
     <row r="1" ht="30" customHeight="true">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2937,13 +2161,13 @@
   <sheetData>
     <row r="1" ht="30" customHeight="true">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3667,7 +2891,7 @@
   <sheetData>
     <row r="1" ht="30" customHeight="true">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4374,157 +3598,37 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>76</v>
-      </c>
-      <c r="R2" t="s">
-        <v>77</v>
-      </c>
-      <c r="S2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T2" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" t="s">
-        <v>80</v>
-      </c>
-      <c r="V2" t="s">
-        <v>81</v>
-      </c>
-      <c r="W2" t="s">
-        <v>82</v>
-      </c>
-      <c r="X2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4547,52 +3651,52 @@
   <sheetData>
     <row r="1" ht="30" customHeight="true">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>122</v>
+        <v>50</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>125</v>
+        <v>53</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -5284,7 +4388,7 @@
     </row>
     <row r="2">
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5295,7 +4399,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5315,34 +4419,34 @@
   <sheetData>
     <row r="1" ht="30" customHeight="true">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>

</xml_diff>